<commit_message>
added new attribute and modified codebase accordint to it also changed the publications.xlsx template into correct one
</commit_message>
<xml_diff>
--- a/backend/template/publications.xlsx
+++ b/backend/template/publications.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDDFCA9-2BED-4E8C-9ADC-8F419126E29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51398431-82B2-45CE-B0C0-0BD69C5C8AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2712" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Publications" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -59,14 +59,29 @@
     <t>Indexation</t>
   </si>
   <si>
-    <t>PDF URL</t>
+    <t>ISSN/ISBN No</t>
+  </si>
+  <si>
+    <t>Journal Link</t>
+  </si>
+  <si>
+    <t>UGC Approved</t>
+  </si>
+  <si>
+    <t>Impact Factor</t>
+  </si>
+  <si>
+    <t>DOI Link</t>
+  </si>
+  <si>
+    <t>Publication Type(Journal Paper/Conference Proceedings)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +94,13 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -121,9 +143,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -465,16 +490,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="A2:B6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" customWidth="1"/>
     <col min="3" max="4" width="30" customWidth="1"/>
     <col min="5" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
@@ -482,58 +507,75 @@
     <col min="10" max="12" width="10" customWidth="1"/>
     <col min="13" max="13" width="15" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
-    <col min="15" max="15" width="40" customWidth="1"/>
+    <col min="15" max="18" width="40" customWidth="1"/>
+    <col min="19" max="19" width="21" customWidth="1"/>
+    <col min="20" max="20" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>